<commit_message>
freeze header line in excel
</commit_message>
<xml_diff>
--- a/data-sample.xlsx
+++ b/data-sample.xlsx
@@ -142,27 +142,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -176,13 +161,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -527,20 +512,21 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -573,19 +559,19 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -593,16 +579,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -611,158 +597,158 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="2"/>
+      <c r="D6" s="3"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D7" s="2"/>
+      <c r="D7" s="3"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="3"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D9" s="2"/>
+      <c r="D9" s="3"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D10" s="2"/>
+      <c r="D10" s="3"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="2"/>
+      <c r="D11" s="3"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="3"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="3"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="3"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="3"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="3"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D17" s="2"/>
+      <c r="D17" s="3"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D18" s="2"/>
+      <c r="D18" s="3"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
+      <c r="D19" s="3"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D20" s="2"/>
+      <c r="D20" s="3"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="3"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C22" s="5"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="3"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="3"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D24" s="2"/>
+      <c r="D24" s="3"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D25" s="2"/>
+      <c r="D25" s="3"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C26" s="5"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="3"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C27" s="5"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="3"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="3"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C29" s="5"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="3"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D30" s="2"/>
+      <c r="D30" s="3"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D31" s="2"/>
+      <c r="D31" s="3"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D32" s="2"/>
+      <c r="D32" s="3"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D33" s="2"/>
+      <c r="D33" s="3"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D34" s="2"/>
+      <c r="D34" s="3"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="2"/>
+      <c r="D35" s="3"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D36" s="2"/>
+      <c r="D36" s="3"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D37" s="2"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D38" s="2"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C39" s="7"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
changes to handle nips2019
</commit_message>
<xml_diff>
--- a/data-sample.xlsx
+++ b/data-sample.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Desktop/mailmerge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Dropbox/nips/2019 Vancouver/TravelApplications/undergraduate-notifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9ACA29-ADB3-E34C-B979-FCD96A744FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26100" yWindow="8140" windowWidth="23240" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="26100" yWindow="8140" windowWidth="23240" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,18 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Redirect</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -59,28 +48,40 @@
     <t>lee@snl.salk.edu</t>
   </si>
   <si>
-    <t>Skiprow</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>Lee Campbell</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
     <t>te.html</t>
   </si>
   <si>
     <t>template.html</t>
+  </si>
+  <si>
+    <t>skiprow</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>redirect</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -182,6 +183,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -508,12 +512,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,65 +538,65 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -753,12 +757,12 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="C3" r:id="rId6"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>